<commit_message>
command parsing for paw detectoin
</commit_message>
<xml_diff>
--- a/cfg/config.xlsx
+++ b/cfg/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auguste.verdier\Desktop\git\OpenField\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auguste.verdier\Desktop\git\OpenField\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2E2C55-6048-4370-A0F5-33A58A4BA2EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67710FF9-55C7-4F1B-B21C-8F8F22945430}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{79FAC723-FA17-42C8-B9C5-2FE53176198B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>anomalies</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>test_rat</t>
+  </si>
+  <si>
+    <t>1_semaine_postL</t>
+  </si>
+  <si>
+    <t>P1B</t>
+  </si>
+  <si>
+    <t>OFGH010144.avi</t>
+  </si>
+  <si>
+    <t>GH010275</t>
+  </si>
+  <si>
+    <t>GH010038</t>
+  </si>
+  <si>
+    <t>GH010047</t>
+  </si>
+  <si>
+    <t>son,,,</t>
   </si>
 </sst>
 </file>
@@ -127,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -208,12 +229,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -223,6 +274,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,7 +606,7 @@
   <dimension ref="A1:N116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +628,7 @@
     <col min="21" max="21" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -606,36 +663,68 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.23611111111111113</v>
+      </c>
+      <c r="I2" s="10">
+        <v>21619</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H3" s="4">
         <v>0.25625000000000003</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>